<commit_message>
Update tracker template to exclude Monday in the count (stock day)
</commit_message>
<xml_diff>
--- a/compliance-tracker-template3.xlsx
+++ b/compliance-tracker-template3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Users\Steve\My Documents\PythonProjects\complanceTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C3750F-4E45-4169-812C-6EF559889ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758F8D7A-A522-48FA-A197-5AF95A12EC2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="11115" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -193,7 +193,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -245,6 +245,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -406,7 +412,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0"/>
@@ -414,8 +420,9 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -479,25 +486,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="20% - Accent1" xfId="4" builtinId="30"/>
+    <cellStyle name="40% - Accent3" xfId="7" builtinId="39"/>
     <cellStyle name="60% - Accent1" xfId="5" builtinId="32"/>
     <cellStyle name="60% - Accent3" xfId="6" builtinId="40"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -505,7 +516,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="3" builtinId="21"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="39">
     <dxf>
       <fill>
         <patternFill>
@@ -601,6 +612,132 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -969,7 +1106,7 @@
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:N1"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -992,62 +1129,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="32" t="s">
+      <c r="C3" s="32"/>
+      <c r="D3" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="33"/>
-      <c r="F3" s="32" t="s">
+      <c r="E3" s="32"/>
+      <c r="F3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="33"/>
-      <c r="H3" s="32" t="s">
+      <c r="G3" s="32"/>
+      <c r="H3" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="33"/>
-      <c r="J3" s="32" t="s">
+      <c r="I3" s="32"/>
+      <c r="J3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="33"/>
-      <c r="L3" s="32" t="s">
+      <c r="K3" s="32"/>
+      <c r="L3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="33"/>
-      <c r="N3" s="32" t="s">
+      <c r="M3" s="32"/>
+      <c r="N3" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="O3" s="33"/>
+      <c r="O3" s="32"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -1065,8 +1202,8 @@
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -1084,8 +1221,8 @@
       <c r="A6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1103,8 +1240,8 @@
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -1122,8 +1259,8 @@
       <c r="A8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1141,8 +1278,8 @@
       <c r="A9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -1160,21 +1297,21 @@
       <c r="A19" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="31"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="35"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8" t="s">
         <v>16</v>
       </c>
       <c r="G19" s="4"/>
-      <c r="J19" s="34" t="s">
+      <c r="J19" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="K19" s="30"/>
-      <c r="L19" s="31"/>
+      <c r="K19" s="34"/>
+      <c r="L19" s="35"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="str">
@@ -1188,8 +1325,8 @@
       <c r="C20" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="16">
-        <f t="array" aca="1" ref="D20" ca="1">SUM(COUNTIF(INDIRECT({"C4","E4","G4","I4","K4","M4","O4"}),"&lt;&gt;"))</f>
+      <c r="D20" s="16" cm="1">
+        <f t="array" aca="1" ref="D20" ca="1">SUM(COUNTIF(INDIRECT({"E4","G4","I4","K4","M4","O4"}),"&lt;&gt;"))</f>
         <v>0</v>
       </c>
       <c r="E20" s="3" t="e">
@@ -1221,7 +1358,7 @@
         <v>18</v>
       </c>
       <c r="D21" s="10" cm="1">
-        <f t="array" aca="1" ref="D21" ca="1">SUM(COUNTIF(INDIRECT({"C5","E5","G5","I5","K5","M5","O5"}),"&lt;&gt;"))</f>
+        <f t="array" aca="1" ref="D21" ca="1">SUM(COUNTIF(INDIRECT({"E5","G5","I5","K5","M5","O5"}),"&lt;&gt;"))</f>
         <v>0</v>
       </c>
       <c r="E21" s="3" t="e">
@@ -1247,8 +1384,8 @@
       <c r="C22" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="19">
-        <f t="array" aca="1" ref="D22" ca="1">SUM(COUNTIF(INDIRECT({"C6","E6","G6","I6","K6","M6","O6"}),"N"))</f>
+      <c r="D22" s="19" cm="1">
+        <f t="array" aca="1" ref="D22" ca="1">SUM(COUNTIF(INDIRECT({"E6","G6","I6","K6","M6","O6"}),"N"))</f>
         <v>0</v>
       </c>
       <c r="E22" s="3" t="e">
@@ -1274,8 +1411,8 @@
       <c r="C23" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="10">
-        <f t="array" aca="1" ref="D23" ca="1">SUM(COUNTIF(INDIRECT({"C7","E7","G7","I7","K7","M7","O7"}),"N"))</f>
+      <c r="D23" s="10" cm="1">
+        <f t="array" aca="1" ref="D23" ca="1">SUM(COUNTIF(INDIRECT({"E7","G7","I7","K7","M7","O7"}),"N"))</f>
         <v>0</v>
       </c>
       <c r="E23" s="3" t="e">
@@ -1295,8 +1432,8 @@
       <c r="C24" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="10">
-        <f t="array" aca="1" ref="D24" ca="1">SUM(COUNTIF(INDIRECT({"C8","E8","G8","I8","K8","M8","O8"}),"N"))</f>
+      <c r="D24" s="10" cm="1">
+        <f t="array" aca="1" ref="D24" ca="1">SUM(COUNTIF(INDIRECT({"E8","G8","I8","K8","M8","O8"}),"N"))</f>
         <v>0</v>
       </c>
       <c r="E24" s="3" t="e">
@@ -1316,8 +1453,8 @@
       <c r="C25" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="10">
-        <f t="array" aca="1" ref="D25" ca="1">SUM(COUNTIF(INDIRECT({"C9","E9","G9","I9","K9","M9","O9"}),"N"))</f>
+      <c r="D25" s="10" cm="1">
+        <f t="array" aca="1" ref="D25" ca="1">SUM(COUNTIF(INDIRECT({"E9","G9","I9","K9","M9","O9"}),"N"))</f>
         <v>0</v>
       </c>
       <c r="E25" s="3" t="e">
@@ -1368,80 +1505,69 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:C9">
-    <cfRule type="expression" dxfId="20" priority="5">
-      <formula>$B4="day-off"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="27">
-      <formula>$C4="N"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="28">
-      <formula>$C4="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="D4:E9">
-    <cfRule type="expression" dxfId="17" priority="22">
+    <cfRule type="expression" dxfId="38" priority="22">
       <formula>$D4="day-off"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="23">
+    <cfRule type="expression" dxfId="37" priority="23">
       <formula>$E4="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="24">
+    <cfRule type="expression" dxfId="36" priority="24">
       <formula>$E4="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:G9">
-    <cfRule type="expression" dxfId="14" priority="19">
+    <cfRule type="expression" dxfId="35" priority="19">
       <formula>$F4="day-off"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="20">
+    <cfRule type="expression" dxfId="34" priority="20">
       <formula>$G4="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="21">
+    <cfRule type="expression" dxfId="33" priority="21">
       <formula>$G4="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:I9">
-    <cfRule type="expression" dxfId="11" priority="16">
+    <cfRule type="expression" dxfId="32" priority="16">
       <formula>$H4="day-off"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="17">
+    <cfRule type="expression" dxfId="31" priority="17">
       <formula>$I4="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="18">
+    <cfRule type="expression" dxfId="30" priority="18">
       <formula>$I4="N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:K9">
-    <cfRule type="expression" dxfId="8" priority="13">
+    <cfRule type="expression" dxfId="29" priority="13">
       <formula>$J4="day-off"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="14">
+    <cfRule type="expression" dxfId="28" priority="14">
       <formula>$K4="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="15">
+    <cfRule type="expression" dxfId="27" priority="15">
       <formula>$K4="N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:M9">
-    <cfRule type="expression" dxfId="5" priority="10">
+    <cfRule type="expression" dxfId="26" priority="10">
       <formula>$L4="day-off"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="11">
+    <cfRule type="expression" dxfId="25" priority="11">
       <formula>$M4="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="12">
+    <cfRule type="expression" dxfId="24" priority="12">
       <formula>$M4="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4:O9">
-    <cfRule type="expression" dxfId="2" priority="7">
+    <cfRule type="expression" dxfId="23" priority="7">
       <formula>$O4="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="8">
+    <cfRule type="expression" dxfId="22" priority="8">
       <formula>$O4="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="9">
+    <cfRule type="expression" dxfId="21" priority="9">
       <formula>$N4="day-off"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>